<commit_message>
feature：ttl2d study play data check
</commit_message>
<xml_diff>
--- a/testCase/ttl2D/ttlstudylist.xlsx
+++ b/testCase/ttl2D/ttlstudylist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12255"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1224,8 +1224,8 @@
   <sheetPr/>
   <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="K164" sqref="K164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>

</xml_diff>